<commit_message>
Updated Exam 2 Up to Problem 3
Answered everything up to problem 3 for exam 2, need to finish the rest of the test.  The deadline has been moved so there are a few more days to work on it.
</commit_message>
<xml_diff>
--- a/Exam2/Problem2/StatisticalAnalysis.xlsx
+++ b/Exam2/Problem2/StatisticalAnalysis.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12210" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12210" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Relative Speedup TSP" sheetId="13" r:id="rId1"/>
@@ -2101,7 +2101,17 @@
     </c:title>
     <c:autoTitleDeleted val="0"/>
     <c:plotArea>
-      <c:layout/>
+      <c:layout>
+        <c:manualLayout>
+          <c:layoutTarget val="inner"/>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="0.13624324944129432"/>
+          <c:y val="7.4818692418889887E-2"/>
+          <c:w val="0.80831140075527164"/>
+          <c:h val="0.86828553607146863"/>
+        </c:manualLayout>
+      </c:layout>
       <c:scatterChart>
         <c:scatterStyle val="smoothMarker"/>
         <c:varyColors val="0"/>
@@ -3010,6 +3020,16 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
+      <c:layout>
+        <c:manualLayout>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="0.52219609183307925"/>
+          <c:y val="0.47147086951556383"/>
+          <c:w val="0.18494677436891305"/>
+          <c:h val="0.17020413472933432"/>
+        </c:manualLayout>
+      </c:layout>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -4750,7 +4770,7 @@
 <chartsheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" xr:uid="{07418FA6-515D-41FA-999E-2F41A34D8848}">
   <sheetPr/>
   <sheetViews>
-    <sheetView zoomScale="117" workbookViewId="0" zoomToFit="1"/>
+    <sheetView zoomScale="123" workbookViewId="0" zoomToFit="1"/>
   </sheetViews>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
@@ -4772,7 +4792,7 @@
 <chartsheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" xr:uid="{2E70E9ED-D03D-490A-867C-2C7EEDADC09E}">
   <sheetPr/>
   <sheetViews>
-    <sheetView zoomScale="117" workbookViewId="0" zoomToFit="1"/>
+    <sheetView tabSelected="1" zoomScale="123" workbookViewId="0" zoomToFit="1"/>
   </sheetViews>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
@@ -4783,7 +4803,7 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:absoluteAnchor>
     <xdr:pos x="0" y="0"/>
-    <xdr:ext cx="8670192" cy="6293013"/>
+    <xdr:ext cx="8673171" cy="6295793"/>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
         <xdr:cNvPr id="2" name="Chart 1">
@@ -4849,7 +4869,7 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:absoluteAnchor>
     <xdr:pos x="0" y="0"/>
-    <xdr:ext cx="8670192" cy="6293013"/>
+    <xdr:ext cx="8673171" cy="6295793"/>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
         <xdr:cNvPr id="2" name="Chart 1">
@@ -5177,7 +5197,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <dimension ref="A1:P27"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="H15" sqref="H15"/>
     </sheetView>
   </sheetViews>
@@ -5260,15 +5280,15 @@
         <v>6.68408E-4</v>
       </c>
       <c r="H2" s="3">
-        <f>B2/C2</f>
+        <f t="shared" ref="H2:H12" si="0">B2/C2</f>
         <v>6.8034924594625235E-2</v>
       </c>
       <c r="I2" s="3">
-        <f>B2/D2</f>
+        <f t="shared" ref="I2:I12" si="1">B2/D2</f>
         <v>3.8709891483270878E-2</v>
       </c>
       <c r="J2" s="3">
-        <f>B2/E2</f>
+        <f t="shared" ref="J2:J12" si="2">B2/E2</f>
         <v>3.401751740158003E-2</v>
       </c>
       <c r="K2" s="3">
@@ -5313,36 +5333,36 @@
         <v>9.5523899999999998E-4</v>
       </c>
       <c r="H3" s="3">
-        <f>B3/C3</f>
+        <f t="shared" si="0"/>
         <v>7.0112989779683416E-2</v>
       </c>
       <c r="I3" s="3">
-        <f>B3/D3</f>
+        <f t="shared" si="1"/>
         <v>4.4280719323254357E-2</v>
       </c>
       <c r="J3" s="3">
-        <f>B3/E3</f>
+        <f t="shared" si="2"/>
         <v>2.9520496307667152E-2</v>
       </c>
       <c r="K3" s="3">
-        <f t="shared" ref="K3:K12" si="0">B3/F3</f>
+        <f t="shared" ref="K3:K12" si="3">B3/F3</f>
         <v>2.7218319185041646E-2</v>
       </c>
       <c r="L3" s="3"/>
       <c r="M3" s="3">
-        <f t="shared" ref="M3:M12" si="1">B3/(1*C3)</f>
+        <f t="shared" ref="M3:M12" si="4">B3/(1*C3)</f>
         <v>7.0112989779683416E-2</v>
       </c>
       <c r="N3" s="3">
-        <f t="shared" ref="N3:N12" si="2">B3/(2*D3)</f>
+        <f t="shared" ref="N3:N12" si="5">B3/(2*D3)</f>
         <v>2.2140359661627178E-2</v>
       </c>
       <c r="O3" s="3">
-        <f t="shared" ref="O3:O12" si="3">B3/(3*E3)</f>
+        <f t="shared" ref="O3:O12" si="6">B3/(3*E3)</f>
         <v>9.8401654358890502E-3</v>
       </c>
       <c r="P3" s="3">
-        <f t="shared" ref="P3:P12" si="4">B3/(4*F3)</f>
+        <f t="shared" ref="P3:P11" si="7">B3/(4*F3)</f>
         <v>6.8045797962604116E-3</v>
       </c>
     </row>
@@ -5366,36 +5386,36 @@
         <v>1.27965E-3</v>
       </c>
       <c r="H4" s="3">
-        <f>B4/C4</f>
+        <f t="shared" si="0"/>
         <v>9.1640460710358265E-2</v>
       </c>
       <c r="I4" s="3">
-        <f>B4/D4</f>
+        <f t="shared" si="1"/>
         <v>6.6667251467118133E-2</v>
       </c>
       <c r="J4" s="3">
-        <f>B4/E4</f>
+        <f t="shared" si="2"/>
         <v>4.5278738296041926E-2</v>
       </c>
       <c r="K4" s="3">
-        <f t="shared" si="0"/>
+        <f t="shared" si="3"/>
         <v>2.9695619896065333E-2</v>
       </c>
       <c r="L4" s="3"/>
       <c r="M4" s="3">
-        <f t="shared" si="1"/>
+        <f t="shared" si="4"/>
         <v>9.1640460710358265E-2</v>
       </c>
       <c r="N4" s="3">
-        <f t="shared" si="2"/>
+        <f t="shared" si="5"/>
         <v>3.3333625733559066E-2</v>
       </c>
       <c r="O4" s="3">
-        <f t="shared" si="3"/>
+        <f t="shared" si="6"/>
         <v>1.509291276534731E-2</v>
       </c>
       <c r="P4" s="3">
-        <f t="shared" si="4"/>
+        <f t="shared" si="7"/>
         <v>7.4239049740163331E-3</v>
       </c>
     </row>
@@ -5419,36 +5439,36 @@
         <v>1.10049E-3</v>
       </c>
       <c r="H5" s="3">
-        <f>B5/C5</f>
+        <f t="shared" si="0"/>
         <v>0.22133332477938839</v>
       </c>
       <c r="I5" s="3">
-        <f>B5/D5</f>
+        <f t="shared" si="1"/>
         <v>9.7081368256362335E-2</v>
       </c>
       <c r="J5" s="3">
-        <f>B5/E5</f>
+        <f t="shared" si="2"/>
         <v>8.1891430951875135E-2</v>
       </c>
       <c r="K5" s="3">
-        <f t="shared" si="0"/>
+        <f t="shared" si="3"/>
         <v>6.2699343019927481E-2</v>
       </c>
       <c r="L5" s="3"/>
       <c r="M5" s="3">
-        <f t="shared" si="1"/>
+        <f t="shared" si="4"/>
         <v>0.22133332477938839</v>
       </c>
       <c r="N5" s="3">
-        <f t="shared" si="2"/>
+        <f t="shared" si="5"/>
         <v>4.8540684128181168E-2</v>
       </c>
       <c r="O5" s="3">
-        <f t="shared" si="3"/>
+        <f t="shared" si="6"/>
         <v>2.7297143650625043E-2</v>
       </c>
       <c r="P5" s="3">
-        <f t="shared" si="4"/>
+        <f t="shared" si="7"/>
         <v>1.567483575498187E-2</v>
       </c>
     </row>
@@ -5472,36 +5492,36 @@
         <v>1.62181E-3</v>
       </c>
       <c r="H6" s="3">
-        <f>B6/C6</f>
+        <f t="shared" si="0"/>
         <v>0.30591249131317538</v>
       </c>
       <c r="I6" s="3">
-        <f>B6/D6</f>
+        <f t="shared" si="1"/>
         <v>0.3421838800146324</v>
       </c>
       <c r="J6" s="3">
-        <f>B6/E6</f>
+        <f t="shared" si="2"/>
         <v>0.3508744510260538</v>
       </c>
       <c r="K6" s="3">
-        <f t="shared" si="0"/>
+        <f t="shared" si="3"/>
         <v>0.27685117245546642</v>
       </c>
       <c r="L6" s="3"/>
       <c r="M6" s="3">
-        <f t="shared" si="1"/>
+        <f t="shared" si="4"/>
         <v>0.30591249131317538</v>
       </c>
       <c r="N6" s="3">
-        <f t="shared" si="2"/>
+        <f t="shared" si="5"/>
         <v>0.1710919400073162</v>
       </c>
       <c r="O6" s="3">
-        <f t="shared" si="3"/>
+        <f t="shared" si="6"/>
         <v>0.11695815034201795</v>
       </c>
       <c r="P6" s="3">
-        <f t="shared" si="4"/>
+        <f t="shared" si="7"/>
         <v>6.9212793113866605E-2</v>
       </c>
     </row>
@@ -5525,36 +5545,36 @@
         <v>3.6047100000000001E-3</v>
       </c>
       <c r="H7" s="3">
-        <f>B7/C7</f>
+        <f t="shared" si="0"/>
         <v>0.35609993510707333</v>
       </c>
       <c r="I7" s="3">
-        <f>B7/D7</f>
+        <f t="shared" si="1"/>
         <v>0.68630925084420724</v>
       </c>
       <c r="J7" s="3">
-        <f>B7/E7</f>
+        <f t="shared" si="2"/>
         <v>0.79655009737628368</v>
       </c>
       <c r="K7" s="3">
-        <f t="shared" si="0"/>
+        <f t="shared" si="3"/>
         <v>1.0960659803423853</v>
       </c>
       <c r="L7" s="3"/>
       <c r="M7" s="3">
-        <f t="shared" si="1"/>
+        <f t="shared" si="4"/>
         <v>0.35609993510707333</v>
       </c>
       <c r="N7" s="3">
-        <f t="shared" si="2"/>
+        <f t="shared" si="5"/>
         <v>0.34315462542210362</v>
       </c>
       <c r="O7" s="3">
-        <f t="shared" si="3"/>
+        <f t="shared" si="6"/>
         <v>0.26551669912542791</v>
       </c>
       <c r="P7" s="3">
-        <f t="shared" si="4"/>
+        <f t="shared" si="7"/>
         <v>0.27401649508559633</v>
       </c>
     </row>
@@ -5578,36 +5598,36 @@
         <v>2.3895E-2</v>
       </c>
       <c r="H8" s="3">
-        <f>B8/C8</f>
+        <f t="shared" si="0"/>
         <v>0.42091566522983059</v>
       </c>
       <c r="I8" s="3">
-        <f>B8/D8</f>
+        <f t="shared" si="1"/>
         <v>0.8399937697476747</v>
       </c>
       <c r="J8" s="3">
-        <f>B8/E8</f>
+        <f t="shared" si="2"/>
         <v>1.245093964999769</v>
       </c>
       <c r="K8" s="3">
-        <f t="shared" si="0"/>
+        <f t="shared" si="3"/>
         <v>1.579870265745972</v>
       </c>
       <c r="L8" s="3"/>
       <c r="M8" s="3">
-        <f t="shared" si="1"/>
+        <f t="shared" si="4"/>
         <v>0.42091566522983059</v>
       </c>
       <c r="N8" s="3">
-        <f t="shared" si="2"/>
+        <f t="shared" si="5"/>
         <v>0.41999688487383735</v>
       </c>
       <c r="O8" s="3">
-        <f t="shared" si="3"/>
+        <f t="shared" si="6"/>
         <v>0.41503132166658974</v>
       </c>
       <c r="P8" s="3">
-        <f t="shared" si="4"/>
+        <f t="shared" si="7"/>
         <v>0.394967566436493</v>
       </c>
     </row>
@@ -5631,36 +5651,36 @@
         <v>0.223387</v>
       </c>
       <c r="H9" s="3">
-        <f>B9/C9</f>
+        <f t="shared" si="0"/>
         <v>0.49496441186389539</v>
       </c>
       <c r="I9" s="3">
-        <f>B9/D9</f>
+        <f t="shared" si="1"/>
         <v>0.96548341454294495</v>
       </c>
       <c r="J9" s="3">
-        <f>B9/E9</f>
+        <f t="shared" si="2"/>
         <v>1.4547493844163433</v>
       </c>
       <c r="K9" s="3">
-        <f t="shared" si="0"/>
+        <f t="shared" si="3"/>
         <v>1.8724769122643663</v>
       </c>
       <c r="L9" s="3"/>
       <c r="M9" s="3">
-        <f t="shared" si="1"/>
+        <f t="shared" si="4"/>
         <v>0.49496441186389539</v>
       </c>
       <c r="N9" s="3">
-        <f t="shared" si="2"/>
+        <f t="shared" si="5"/>
         <v>0.48274170727147248</v>
       </c>
       <c r="O9" s="3">
-        <f t="shared" si="3"/>
+        <f t="shared" si="6"/>
         <v>0.48491646147211442</v>
       </c>
       <c r="P9" s="3">
-        <f t="shared" si="4"/>
+        <f t="shared" si="7"/>
         <v>0.46811922806609157</v>
       </c>
     </row>
@@ -5684,36 +5704,36 @@
         <v>2.3794300000000002</v>
       </c>
       <c r="H10" s="3">
-        <f>B10/C10</f>
+        <f t="shared" si="0"/>
         <v>0.53181472737684432</v>
       </c>
       <c r="I10" s="3">
-        <f>B10/D10</f>
+        <f t="shared" si="1"/>
         <v>1.0302980938162443</v>
       </c>
       <c r="J10" s="3">
-        <f>B10/E10</f>
+        <f t="shared" si="2"/>
         <v>1.5863029094649683</v>
       </c>
       <c r="K10" s="3">
-        <f t="shared" si="0"/>
+        <f t="shared" si="3"/>
         <v>2.099834834393111</v>
       </c>
       <c r="L10" s="3"/>
       <c r="M10" s="3">
-        <f t="shared" si="1"/>
+        <f t="shared" si="4"/>
         <v>0.53181472737684432</v>
       </c>
       <c r="N10" s="3">
-        <f t="shared" si="2"/>
+        <f t="shared" si="5"/>
         <v>0.51514904690812213</v>
       </c>
       <c r="O10" s="3">
-        <f t="shared" si="3"/>
+        <f t="shared" si="6"/>
         <v>0.52876763648832281</v>
       </c>
       <c r="P10" s="3">
-        <f t="shared" si="4"/>
+        <f t="shared" si="7"/>
         <v>0.52495870859827776</v>
       </c>
     </row>
@@ -5737,36 +5757,36 @@
         <v>28.880199999999999</v>
       </c>
       <c r="H11" s="3">
-        <f>B11/C11</f>
+        <f t="shared" si="0"/>
         <v>0.56981143691403846</v>
       </c>
       <c r="I11" s="3">
-        <f>B11/D11</f>
+        <f t="shared" si="1"/>
         <v>1.14270621684163</v>
       </c>
       <c r="J11" s="3">
-        <f>B11/E11</f>
+        <f t="shared" si="2"/>
         <v>1.715016689916961</v>
       </c>
       <c r="K11" s="3">
-        <f t="shared" si="0"/>
+        <f t="shared" si="3"/>
         <v>2.2433605030436081</v>
       </c>
       <c r="L11" s="3"/>
       <c r="M11" s="3">
-        <f t="shared" si="1"/>
+        <f t="shared" si="4"/>
         <v>0.56981143691403846</v>
       </c>
       <c r="N11" s="3">
-        <f t="shared" si="2"/>
+        <f t="shared" si="5"/>
         <v>0.57135310842081499</v>
       </c>
       <c r="O11" s="3">
-        <f t="shared" si="3"/>
+        <f t="shared" si="6"/>
         <v>0.57167222997232037</v>
       </c>
       <c r="P11" s="3">
-        <f t="shared" si="4"/>
+        <f t="shared" si="7"/>
         <v>0.56084012576090203</v>
       </c>
     </row>
@@ -5790,32 +5810,32 @@
         <v>373.61599999999999</v>
       </c>
       <c r="H12" s="3">
-        <f>B12/C12</f>
+        <f t="shared" si="0"/>
         <v>0.59112909018486226</v>
       </c>
       <c r="I12" s="3">
-        <f>B12/D12</f>
+        <f t="shared" si="1"/>
         <v>1.2103940869574519</v>
       </c>
       <c r="J12" s="3">
-        <f>B12/E12</f>
+        <f t="shared" si="2"/>
         <v>1.8314184849128556</v>
       </c>
       <c r="K12" s="3">
-        <f t="shared" si="0"/>
+        <f t="shared" si="3"/>
         <v>2.4229717142734786</v>
       </c>
       <c r="L12" s="3"/>
       <c r="M12" s="3">
-        <f t="shared" si="1"/>
+        <f t="shared" si="4"/>
         <v>0.59112909018486226</v>
       </c>
       <c r="N12" s="3">
-        <f t="shared" si="2"/>
+        <f t="shared" si="5"/>
         <v>0.60519704347872594</v>
       </c>
       <c r="O12" s="3">
-        <f t="shared" si="3"/>
+        <f t="shared" si="6"/>
         <v>0.61047282830428518</v>
       </c>
       <c r="P12" s="3">

</xml_diff>